<commit_message>
Physics notes week 2
</commit_message>
<xml_diff>
--- a/FrameworlPatternExamples/FrameworlPatternExamples/Book1.xlsx
+++ b/FrameworlPatternExamples/FrameworlPatternExamples/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2024-2025\GDP202425\FrameworlPatternExamples\FrameworlPatternExamples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD84662-FE32-4A57-A544-D704B8FB821F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A037EB70-6D59-4575-82C2-D6ED221C33E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2C3F7CFF-D097-4D26-86EA-065730562E6B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2C3F7CFF-D097-4D26-86EA-065730562E6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Monster</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>MonsterWeaponVehicleJetpackTF</t>
+  </si>
+  <si>
+    <t>IsRanged</t>
   </si>
 </sst>
 </file>
@@ -503,22 +506,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727C6F6D-ABEB-4367-8B77-CD1DE3ABBEE4}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E6" sqref="E6:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="1" max="2" width="12.21875" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,27 +528,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -568,8 +570,11 @@
       <c r="G6" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -589,8 +594,11 @@
       <c r="G7" s="4">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -606,8 +614,11 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -615,7 +626,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4" t="s">
@@ -623,8 +634,11 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -640,8 +654,11 @@
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -657,6 +674,9 @@
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>